<commit_message>
comparison table is updated with Efficient Kruskal weights and time complexity
</commit_message>
<xml_diff>
--- a/Assignment_2_Comparison.xlsx
+++ b/Assignment_2_Comparison.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlisaThings\Documents\GitHub\algo2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimad\dev\python\Jupyter_notebook\Advanced algorithms\Exercise 1\algo2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0EC61E-CEFE-436D-8328-AE0A25A03A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18030" windowHeight="5520"/>
+    <workbookView xWindow="13980" yWindow="2565" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -92,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -788,11 +799,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,8 +812,7 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -878,11 +888,15 @@
         <f>(C3-B3)/B3</f>
         <v>2.7578891540705381</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="F3" s="9">
+        <v>10130</v>
+      </c>
+      <c r="G3" s="10">
+        <v>5631700</v>
+      </c>
       <c r="H3" s="11">
         <f>(F3-B3)/B3</f>
-        <v>-1</v>
+        <v>0.34314505436223813</v>
       </c>
       <c r="I3" s="12">
         <v>8955</v>
@@ -912,11 +926,15 @@
         <f>(C4-B4)/B4</f>
         <v>1.1959073126692747</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="F4" s="17">
+        <v>3583</v>
+      </c>
+      <c r="G4" s="18">
+        <v>472100</v>
+      </c>
       <c r="H4" s="19">
         <f t="shared" ref="H4:H15" si="0">(F4-B4)/B4</f>
-        <v>-1</v>
+        <v>7.8242551910923858E-2</v>
       </c>
       <c r="I4" s="20">
         <v>3424</v>
@@ -946,11 +964,15 @@
         <f t="shared" ref="E5:E15" si="2">(C5-B5)/B5</f>
         <v>6.958333333333333</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="17">
+        <v>8398</v>
+      </c>
+      <c r="G5" s="18">
+        <v>42477400</v>
+      </c>
       <c r="H5" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.28645833333333331</v>
       </c>
       <c r="I5" s="20">
         <v>8229</v>
@@ -980,11 +1002,15 @@
         <f t="shared" si="2"/>
         <v>11.742957545283126</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="F6" s="17">
+        <v>45261</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1211420700</v>
+      </c>
       <c r="H6" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.29309753728358379</v>
       </c>
       <c r="I6" s="20">
         <v>41930</v>
@@ -1014,11 +1040,15 @@
         <f t="shared" si="2"/>
         <v>29.138658481320803</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="17">
+        <v>24977771</v>
+      </c>
+      <c r="G7" s="18">
+        <v>10492520200</v>
+      </c>
       <c r="H7" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.3385953184211869</v>
       </c>
       <c r="I7" s="20">
         <v>24491641</v>
@@ -1048,11 +1078,15 @@
         <f t="shared" si="2"/>
         <v>2.6572769953051645</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+      <c r="F8" s="17">
+        <v>586</v>
+      </c>
+      <c r="G8" s="18">
+        <v>20189200</v>
+      </c>
       <c r="H8" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.37558685446009388</v>
       </c>
       <c r="I8" s="20">
         <v>533</v>
@@ -1082,11 +1116,15 @@
         <f t="shared" si="2"/>
         <v>5.8094123505976096</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="17">
+        <v>52476</v>
+      </c>
+      <c r="G9" s="18">
+        <v>107441700</v>
+      </c>
       <c r="H9" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.30667330677290838</v>
       </c>
       <c r="I9" s="20">
         <v>51136</v>
@@ -1116,11 +1154,15 @@
         <f t="shared" si="2"/>
         <v>8.7914592650926426</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="17">
+        <v>177544</v>
+      </c>
+      <c r="G10" s="18">
+        <v>129493500</v>
+      </c>
       <c r="H10" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.31902943492667268</v>
       </c>
       <c r="I10" s="20">
         <v>162905</v>
@@ -1150,11 +1192,15 @@
         <f t="shared" si="2"/>
         <v>6.2635090686965507</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="F11" s="17">
+        <v>27749</v>
+      </c>
+      <c r="G11" s="18">
+        <v>15979800</v>
+      </c>
       <c r="H11" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.30387181655859413</v>
       </c>
       <c r="I11" s="20">
         <v>26957</v>
@@ -1184,11 +1230,15 @@
         <f t="shared" si="2"/>
         <v>6.8688832534986384</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
+      <c r="F12" s="17">
+        <v>28140</v>
+      </c>
+      <c r="G12" s="18">
+        <v>14318000</v>
+      </c>
       <c r="H12" s="19">
         <f>(F12-B12)/B12</f>
-        <v>-1</v>
+        <v>0.32149901380670609</v>
       </c>
       <c r="I12" s="20">
         <v>27072</v>
@@ -1218,11 +1268,15 @@
         <f t="shared" si="2"/>
         <v>14.089960218992477</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="17">
+        <v>68999</v>
+      </c>
+      <c r="G13" s="18">
+        <v>824264600</v>
+      </c>
       <c r="H13" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.35883650399779432</v>
       </c>
       <c r="I13" s="20">
         <v>65497</v>
@@ -1252,11 +1306,15 @@
         <f t="shared" si="2"/>
         <v>0.78451669339553876</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="17">
+        <v>7986</v>
+      </c>
+      <c r="G14" s="18">
+        <v>3415300</v>
+      </c>
       <c r="H14" s="19">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.16430966613208922</v>
       </c>
       <c r="I14" s="20">
         <v>8175</v>
@@ -1286,11 +1344,15 @@
         <f t="shared" si="2"/>
         <v>1.4524454584343363</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="25">
+        <v>8359</v>
+      </c>
+      <c r="G15" s="26">
+        <v>467500</v>
+      </c>
       <c r="H15" s="27">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0.19192927420504777</v>
       </c>
       <c r="I15" s="28">
         <v>8781</v>

</xml_diff>